<commit_message>
attempting to get past batch_config sheet now found in workbook
</commit_message>
<xml_diff>
--- a/BatchFactory/cariboo_jobs.xlsx
+++ b/BatchFactory/cariboo_jobs.xlsx
@@ -58,6 +58,9 @@
     <t>run_as_fcbc</t>
   </si>
   <si>
+    <t>batch_condition</t>
+  </si>
+  <si>
     <t>Cariboo</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
   </si>
   <si>
     <t>Omineca</t>
-  </si>
-  <si>
-    <t>batch_condition</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,26 +754,26 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="14" t="b">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="14" t="b">
         <v>0</v>
@@ -798,29 +798,29 @@
     </row>
     <row r="3" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>17</v>
       </c>
       <c r="J3" s="14" t="b">
         <v>0</v>
@@ -836,19 +836,19 @@
     </row>
     <row r="4" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -857,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="14" t="b">
         <v>0</v>
@@ -868,7 +868,6 @@
       <c r="L4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="M4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -899,7 +898,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" t="b">
         <v>1</v>
@@ -907,7 +906,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -915,32 +914,32 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>